<commit_message>
Fixed some bugs involving pandas and data output
</commit_message>
<xml_diff>
--- a/tests/sample_input_data.xlsx
+++ b/tests/sample_input_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\University\Grad School\University of Toronto\Research\python\dataImportandPlottingToolbox\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen\Documents\University\Grad School\University of Toronto\Research\python\FermAT\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="223">
   <si>
     <t>OD600</t>
   </si>
@@ -1011,15 +1011,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O210"/>
+  <dimension ref="A1:O209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="L211" sqref="L211"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="J207" sqref="J207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
@@ -8345,15 +8347,15 @@
         <v>0</v>
       </c>
       <c r="O156">
-        <v>0.14977170504957463</v>
+        <v>0.24271500306581498</v>
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B157">
-        <v>0</v>
+        <v>28.428714999344336</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -8377,7 +8379,7 @@
         <v>0</v>
       </c>
       <c r="J157">
-        <v>0</v>
+        <v>2.726287652875584E-2</v>
       </c>
       <c r="K157">
         <v>0</v>
@@ -8392,18 +8394,18 @@
         <v>0</v>
       </c>
       <c r="O157">
-        <v>0.24271500306581498</v>
+        <v>0.45999899419884321</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B158">
-        <v>28.428714999344336</v>
+        <v>27.200904529975315</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>2.3194275420636984E-2</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -8418,13 +8420,13 @@
         <v>0</v>
       </c>
       <c r="H158">
-        <v>0</v>
+        <v>0.35184558844183789</v>
       </c>
       <c r="I158">
         <v>0</v>
       </c>
       <c r="J158">
-        <v>2.726287652875584E-2</v>
+        <v>0.16501394246602413</v>
       </c>
       <c r="K158">
         <v>0</v>
@@ -8433,24 +8435,24 @@
         <v>0</v>
       </c>
       <c r="M158">
-        <v>0</v>
+        <v>9.7595868293103485E-3</v>
       </c>
       <c r="N158">
         <v>0</v>
       </c>
       <c r="O158">
-        <v>0.45999899419884321</v>
+        <v>0.92715936065265681</v>
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B159">
-        <v>27.200904529975315</v>
+        <v>25.356899168007505</v>
       </c>
       <c r="C159">
-        <v>2.3194275420636984E-2</v>
+        <v>3.7394708712119348E-2</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -8465,39 +8467,39 @@
         <v>0</v>
       </c>
       <c r="H159">
-        <v>0.35184558844183789</v>
+        <v>0.57315051155429564</v>
       </c>
       <c r="I159">
         <v>0</v>
       </c>
       <c r="J159">
-        <v>0.16501394246602413</v>
+        <v>0.23631739209385585</v>
       </c>
       <c r="K159">
-        <v>0</v>
+        <v>2.9176551639578614E-2</v>
       </c>
       <c r="L159">
-        <v>0</v>
+        <v>3.2566203004239401E-3</v>
       </c>
       <c r="M159">
-        <v>9.7595868293103485E-3</v>
+        <v>4.1900964437695705E-2</v>
       </c>
       <c r="N159">
         <v>0</v>
       </c>
       <c r="O159">
-        <v>0.92715936065265681</v>
+        <v>1.6885900555849649</v>
       </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B160">
-        <v>25.356899168007505</v>
+        <v>23.396581149221191</v>
       </c>
       <c r="C160">
-        <v>3.7394708712119348E-2</v>
+        <v>0.15147861040650673</v>
       </c>
       <c r="D160">
         <v>0</v>
@@ -8512,39 +8514,39 @@
         <v>0</v>
       </c>
       <c r="H160">
-        <v>0.57315051155429564</v>
+        <v>0.67742805507862303</v>
       </c>
       <c r="I160">
         <v>0</v>
       </c>
       <c r="J160">
-        <v>0.23631739209385585</v>
+        <v>0.13765781564389049</v>
       </c>
       <c r="K160">
-        <v>2.9176551639578614E-2</v>
+        <v>7.4376225565992535E-2</v>
       </c>
       <c r="L160">
-        <v>3.2566203004239401E-3</v>
+        <v>0</v>
       </c>
       <c r="M160">
-        <v>4.1900964437695705E-2</v>
+        <v>6.715061898745428E-2</v>
       </c>
       <c r="N160">
         <v>0</v>
       </c>
       <c r="O160">
-        <v>1.6885900555849649</v>
+        <v>3.2453715503303222</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B161">
-        <v>23.396581149221191</v>
+        <v>19.123391170397039</v>
       </c>
       <c r="C161">
-        <v>0.15147861040650673</v>
+        <v>0.22044856533244453</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -8559,39 +8561,39 @@
         <v>0</v>
       </c>
       <c r="H161">
-        <v>0.67742805507862303</v>
+        <v>0.90097288129749364</v>
       </c>
       <c r="I161">
-        <v>0</v>
+        <v>0.22298525325447888</v>
       </c>
       <c r="J161">
-        <v>0.13765781564389049</v>
+        <v>0.62292391253612345</v>
       </c>
       <c r="K161">
-        <v>7.4376225565992535E-2</v>
+        <v>0.47053141264429638</v>
       </c>
       <c r="L161">
-        <v>0</v>
+        <v>0.29426919542705671</v>
       </c>
       <c r="M161">
-        <v>6.715061898745428E-2</v>
+        <v>0.43589093801904455</v>
       </c>
       <c r="N161">
         <v>0</v>
       </c>
       <c r="O161">
-        <v>3.2453715503303222</v>
+        <v>5.3771826439194639</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B162">
-        <v>19.123391170397039</v>
+        <v>42.783204465354039</v>
       </c>
       <c r="C162">
-        <v>0.22044856533244453</v>
+        <v>0.24600848188806509</v>
       </c>
       <c r="D162">
         <v>0</v>
@@ -8606,39 +8608,39 @@
         <v>0</v>
       </c>
       <c r="H162">
-        <v>0.90097288129749364</v>
+        <v>0.67618279976736495</v>
       </c>
       <c r="I162">
-        <v>0.22298525325447888</v>
+        <v>0.19958484636962875</v>
       </c>
       <c r="J162">
-        <v>0.62292391253612345</v>
+        <v>0.54757901609918891</v>
       </c>
       <c r="K162">
-        <v>0.47053141264429638</v>
+        <v>0.27363402237938828</v>
       </c>
       <c r="L162">
-        <v>0.29426919542705671</v>
+        <v>0.31264928530811215</v>
       </c>
       <c r="M162">
-        <v>0.43589093801904455</v>
+        <v>0.3823367219605166</v>
       </c>
       <c r="N162">
         <v>0</v>
       </c>
       <c r="O162">
-        <v>5.3771826439194639</v>
+        <v>5.3391426026155697</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B163">
-        <v>42.783204465354039</v>
+        <v>47.920212511415421</v>
       </c>
       <c r="C163">
-        <v>0.24600848188806509</v>
+        <v>9.1217194055802905E-2</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -8653,39 +8655,39 @@
         <v>0</v>
       </c>
       <c r="H163">
-        <v>0.67618279976736495</v>
+        <v>0.98361781929505232</v>
       </c>
       <c r="I163">
-        <v>0.19958484636962875</v>
+        <v>0.47000321694098085</v>
       </c>
       <c r="J163">
-        <v>0.54757901609918891</v>
+        <v>0.85482086102183696</v>
       </c>
       <c r="K163">
-        <v>0.27363402237938828</v>
+        <v>1.081963864735378</v>
       </c>
       <c r="L163">
-        <v>0.31264928530811215</v>
+        <v>0.72472784577067695</v>
       </c>
       <c r="M163">
-        <v>0.3823367219605166</v>
+        <v>0.90401492777822556</v>
       </c>
       <c r="N163">
         <v>0</v>
       </c>
       <c r="O163">
-        <v>5.3391426026155697</v>
+        <v>5.2184680356032844</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B164">
-        <v>47.920212511415421</v>
+        <v>46.048973750927189</v>
       </c>
       <c r="C164">
-        <v>9.1217194055802905E-2</v>
+        <v>0</v>
       </c>
       <c r="D164">
         <v>0</v>
@@ -8700,36 +8702,36 @@
         <v>0</v>
       </c>
       <c r="H164">
-        <v>0.98361781929505232</v>
+        <v>0.87673657781166003</v>
       </c>
       <c r="I164">
-        <v>0.47000321694098085</v>
+        <v>0.58119319898662003</v>
       </c>
       <c r="J164">
-        <v>0.85482086102183696</v>
+        <v>0.97794648380310312</v>
       </c>
       <c r="K164">
-        <v>1.081963864735378</v>
+        <v>0.75497497331767338</v>
       </c>
       <c r="L164">
-        <v>0.72472784577067695</v>
+        <v>0.86782128591369168</v>
       </c>
       <c r="M164">
-        <v>0.90401492777822556</v>
+        <v>1.465438824242689</v>
       </c>
       <c r="N164">
         <v>0</v>
       </c>
       <c r="O164">
-        <v>5.2184680356032844</v>
+        <v>4.4579247848171839</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B165">
-        <v>46.048973750927189</v>
+        <v>36.696837326347733</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -8747,36 +8749,36 @@
         <v>0</v>
       </c>
       <c r="H165">
-        <v>0.87673657781166003</v>
+        <v>0.95887521857248792</v>
       </c>
       <c r="I165">
-        <v>0.58119319898662003</v>
+        <v>0.81313389137089043</v>
       </c>
       <c r="J165">
-        <v>0.97794648380310312</v>
+        <v>1.1860794618816508</v>
       </c>
       <c r="K165">
-        <v>0.75497497331767338</v>
+        <v>0.89344478998205445</v>
       </c>
       <c r="L165">
-        <v>0.86782128591369168</v>
+        <v>0.85834942842389161</v>
       </c>
       <c r="M165">
-        <v>1.465438824242689</v>
+        <v>2.0941326583293982</v>
       </c>
       <c r="N165">
         <v>0</v>
       </c>
       <c r="O165">
-        <v>4.4579247848171839</v>
+        <v>4.3770611569154791</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B166">
-        <v>36.696837326347733</v>
+        <v>0</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -8794,28 +8796,28 @@
         <v>0</v>
       </c>
       <c r="H166">
-        <v>0.95887521857248792</v>
+        <v>0</v>
       </c>
       <c r="I166">
-        <v>0.81313389137089043</v>
+        <v>0</v>
       </c>
       <c r="J166">
-        <v>1.1860794618816508</v>
+        <v>0</v>
       </c>
       <c r="K166">
-        <v>0.89344478998205445</v>
+        <v>0</v>
       </c>
       <c r="L166">
-        <v>0.85834942842389161</v>
+        <v>0</v>
       </c>
       <c r="M166">
-        <v>2.0941326583293982</v>
+        <v>0</v>
       </c>
       <c r="N166">
         <v>0</v>
       </c>
       <c r="O166">
-        <v>4.3770611569154791</v>
+        <v>0.19839558540886784</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.45">
@@ -8862,15 +8864,15 @@
         <v>0</v>
       </c>
       <c r="O167">
-        <v>0.19839558540886784</v>
+        <v>0.28816926804258314</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B168">
-        <v>0</v>
+        <v>26.210711440416187</v>
       </c>
       <c r="C168">
         <v>0</v>
@@ -8894,7 +8896,7 @@
         <v>0</v>
       </c>
       <c r="J168">
-        <v>0</v>
+        <v>2.2828721062786262E-2</v>
       </c>
       <c r="K168">
         <v>0</v>
@@ -8909,18 +8911,18 @@
         <v>0</v>
       </c>
       <c r="O168">
-        <v>0.28816926804258314</v>
+        <v>0.50879774293282409</v>
       </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B169">
-        <v>26.210711440416187</v>
+        <v>30.488156600878433</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>2.8689321614988109E-2</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -8935,13 +8937,13 @@
         <v>0</v>
       </c>
       <c r="H169">
-        <v>0</v>
+        <v>0.43122666288151518</v>
       </c>
       <c r="I169">
         <v>0</v>
       </c>
       <c r="J169">
-        <v>2.2828721062786262E-2</v>
+        <v>0.15478889768656159</v>
       </c>
       <c r="K169">
         <v>0</v>
@@ -8956,18 +8958,18 @@
         <v>0</v>
       </c>
       <c r="O169">
-        <v>0.50879774293282409</v>
+        <v>1.264799702961529</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B170">
-        <v>30.488156600878433</v>
+        <v>27.166575315254747</v>
       </c>
       <c r="C170">
-        <v>2.8689321614988109E-2</v>
+        <v>5.6610460511909183E-2</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -8982,39 +8984,39 @@
         <v>0</v>
       </c>
       <c r="H170">
-        <v>0.43122666288151518</v>
+        <v>0.57646630540589217</v>
       </c>
       <c r="I170">
         <v>0</v>
       </c>
       <c r="J170">
-        <v>0.15478889768656159</v>
+        <v>0.23777615957797937</v>
       </c>
       <c r="K170">
-        <v>0</v>
+        <v>3.2079268871719364E-2</v>
       </c>
       <c r="L170">
         <v>0</v>
       </c>
       <c r="M170">
-        <v>0</v>
+        <v>5.2654594269875191E-2</v>
       </c>
       <c r="N170">
         <v>0</v>
       </c>
       <c r="O170">
-        <v>1.264799702961529</v>
+        <v>2.3560223866467136</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B171">
-        <v>27.166575315254747</v>
+        <v>24.785949276769905</v>
       </c>
       <c r="C171">
-        <v>5.6610460511909183E-2</v>
+        <v>0.15703367867823609</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -9029,39 +9031,39 @@
         <v>0</v>
       </c>
       <c r="H171">
-        <v>0.57646630540589217</v>
+        <v>0.84470930262009747</v>
       </c>
       <c r="I171">
         <v>0</v>
       </c>
       <c r="J171">
-        <v>0.23777615957797937</v>
+        <v>0.13526230526909322</v>
       </c>
       <c r="K171">
-        <v>3.2079268871719364E-2</v>
+        <v>9.8090908726610471E-2</v>
       </c>
       <c r="L171">
         <v>0</v>
       </c>
       <c r="M171">
-        <v>5.2654594269875191E-2</v>
+        <v>0.11901854856539847</v>
       </c>
       <c r="N171">
         <v>0</v>
       </c>
       <c r="O171">
-        <v>2.3560223866467136</v>
+        <v>4.0108155464101882</v>
       </c>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B172">
-        <v>24.785949276769905</v>
+        <v>14.020345630622408</v>
       </c>
       <c r="C172">
-        <v>0.15703367867823609</v>
+        <v>0.18338333956402442</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -9076,39 +9078,39 @@
         <v>0</v>
       </c>
       <c r="H172">
-        <v>0.84470930262009747</v>
+        <v>0.86937005453584748</v>
       </c>
       <c r="I172">
-        <v>0</v>
+        <v>0.23818354381210421</v>
       </c>
       <c r="J172">
-        <v>0.13526230526909322</v>
+        <v>0.77063603233654498</v>
       </c>
       <c r="K172">
-        <v>9.8090908726610471E-2</v>
+        <v>0.4928697060431429</v>
       </c>
       <c r="L172">
-        <v>0</v>
+        <v>0.64416526185391954</v>
       </c>
       <c r="M172">
-        <v>0.11901854856539847</v>
+        <v>0.5069068947054588</v>
       </c>
       <c r="N172">
         <v>0</v>
       </c>
       <c r="O172">
-        <v>4.0108155464101882</v>
+        <v>6.0576031542629982</v>
       </c>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B173">
-        <v>14.020345630622408</v>
+        <v>41.963513241641017</v>
       </c>
       <c r="C173">
-        <v>0.18338333956402442</v>
+        <v>0.20977635404843351</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -9123,39 +9125,39 @@
         <v>0</v>
       </c>
       <c r="H173">
-        <v>0.86937005453584748</v>
+        <v>0.74393685810075749</v>
       </c>
       <c r="I173">
-        <v>0.23818354381210421</v>
+        <v>0.22150348127025926</v>
       </c>
       <c r="J173">
-        <v>0.77063603233654498</v>
+        <v>0.72077960948721165</v>
       </c>
       <c r="K173">
-        <v>0.4928697060431429</v>
+        <v>0.45079457485114444</v>
       </c>
       <c r="L173">
-        <v>0.64416526185391954</v>
+        <v>0.62622872466825497</v>
       </c>
       <c r="M173">
-        <v>0.5069068947054588</v>
+        <v>0.52686595545976</v>
       </c>
       <c r="N173">
         <v>0</v>
       </c>
       <c r="O173">
-        <v>6.0576031542629982</v>
+        <v>5.7115012870102415</v>
       </c>
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B174">
-        <v>41.963513241641017</v>
+        <v>39.499278943357439</v>
       </c>
       <c r="C174">
-        <v>0.20977635404843351</v>
+        <v>2.1820076099513093E-2</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -9170,39 +9172,39 @@
         <v>0</v>
       </c>
       <c r="H174">
-        <v>0.74393685810075749</v>
+        <v>0.94208939986753792</v>
       </c>
       <c r="I174">
-        <v>0.22150348127025926</v>
+        <v>0.45025135263218713</v>
       </c>
       <c r="J174">
-        <v>0.72077960948721165</v>
+        <v>0.70218171636319726</v>
       </c>
       <c r="K174">
-        <v>0.45079457485114444</v>
+        <v>0.79743096556173865</v>
       </c>
       <c r="L174">
-        <v>0.62622872466825497</v>
+        <v>1.0808986028628471</v>
       </c>
       <c r="M174">
-        <v>0.52686595545976</v>
+        <v>0.88166297696335316</v>
       </c>
       <c r="N174">
         <v>0</v>
       </c>
       <c r="O174">
-        <v>5.7115012870102415</v>
+        <v>5.9502650635308214</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B175">
-        <v>39.499278943357439</v>
+        <v>35.691159213772508</v>
       </c>
       <c r="C175">
-        <v>2.1820076099513093E-2</v>
+        <v>0</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -9217,36 +9219,36 @@
         <v>0</v>
       </c>
       <c r="H175">
-        <v>0.94208939986753792</v>
+        <v>0.92179866292826851</v>
       </c>
       <c r="I175">
-        <v>0.45025135263218713</v>
+        <v>0.59413649814594571</v>
       </c>
       <c r="J175">
-        <v>0.70218171636319726</v>
+        <v>0.57995649991007026</v>
       </c>
       <c r="K175">
-        <v>0.79743096556173865</v>
+        <v>0.98469838109258723</v>
       </c>
       <c r="L175">
-        <v>1.0808986028628471</v>
+        <v>1.5691838706186596</v>
       </c>
       <c r="M175">
-        <v>0.88166297696335316</v>
+        <v>1.192902617256095</v>
       </c>
       <c r="N175">
         <v>0</v>
       </c>
       <c r="O175">
-        <v>5.9502650635308214</v>
+        <v>5.5225275359599904</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B176">
-        <v>35.691159213772508</v>
+        <v>39.262442284367303</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -9264,36 +9266,36 @@
         <v>0</v>
       </c>
       <c r="H176">
-        <v>0.92179866292826851</v>
+        <v>0.87485561878762985</v>
       </c>
       <c r="I176">
-        <v>0.59413649814594571</v>
+        <v>0.82810782726369692</v>
       </c>
       <c r="J176">
-        <v>0.57995649991007026</v>
+        <v>0.57024439837900442</v>
       </c>
       <c r="K176">
-        <v>0.98469838109258723</v>
+        <v>1.2762860100959026</v>
       </c>
       <c r="L176">
-        <v>1.5691838706186596</v>
+        <v>2.1067085510888228</v>
       </c>
       <c r="M176">
-        <v>1.192902617256095</v>
+        <v>1.5909530600597361</v>
       </c>
       <c r="N176">
         <v>0</v>
       </c>
       <c r="O176">
-        <v>5.5225275359599904</v>
+        <v>4.8295154702838037</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>131</v>
+        <v>190</v>
       </c>
       <c r="B177">
-        <v>39.262442284367303</v>
+        <v>0</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -9311,33 +9313,33 @@
         <v>0</v>
       </c>
       <c r="H177">
-        <v>0.87485561878762985</v>
+        <v>0</v>
       </c>
       <c r="I177">
-        <v>0.82810782726369692</v>
+        <v>0</v>
       </c>
       <c r="J177">
-        <v>0.57024439837900442</v>
+        <v>0</v>
       </c>
       <c r="K177">
-        <v>1.2762860100959026</v>
+        <v>0</v>
       </c>
       <c r="L177">
-        <v>2.1067085510888228</v>
+        <v>0</v>
       </c>
       <c r="M177">
-        <v>1.5909530600597361</v>
+        <v>0</v>
       </c>
       <c r="N177">
         <v>0</v>
       </c>
       <c r="O177">
-        <v>4.8295154702838037</v>
+        <v>0.16602462016966377</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -9379,15 +9381,15 @@
         <v>0</v>
       </c>
       <c r="O178">
-        <v>0.16602462016966377</v>
+        <v>0.20677910561152099</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B179">
-        <v>0</v>
+        <v>32.616358749104343</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -9426,18 +9428,18 @@
         <v>0</v>
       </c>
       <c r="O179">
-        <v>0.20677910561152099</v>
+        <v>0.23527309636057306</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B180">
-        <v>32.616358749104343</v>
+        <v>31.792176921235782</v>
       </c>
       <c r="C180">
-        <v>0</v>
+        <v>1.410715185241304E-2</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -9452,7 +9454,7 @@
         <v>0</v>
       </c>
       <c r="H180">
-        <v>0</v>
+        <v>0.31836657709076677</v>
       </c>
       <c r="I180">
         <v>0</v>
@@ -9473,18 +9475,18 @@
         <v>0</v>
       </c>
       <c r="O180">
-        <v>0.23527309636057306</v>
+        <v>0.72329210403087296</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B181">
-        <v>31.792176921235782</v>
+        <v>30.471930695350832</v>
       </c>
       <c r="C181">
-        <v>1.410715185241304E-2</v>
+        <v>0.10427530425080749</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -9499,7 +9501,7 @@
         <v>0</v>
       </c>
       <c r="H181">
-        <v>0.31836657709076677</v>
+        <v>0.48870582503369758</v>
       </c>
       <c r="I181">
         <v>0</v>
@@ -9520,18 +9522,18 @@
         <v>0</v>
       </c>
       <c r="O181">
-        <v>0.72329210403087296</v>
+        <v>1.0103885507437727</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B182">
-        <v>30.471930695350832</v>
+        <v>28.753646018813022</v>
       </c>
       <c r="C182">
-        <v>0.10427530425080749</v>
+        <v>0.26638251944622743</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -9546,7 +9548,7 @@
         <v>0</v>
       </c>
       <c r="H182">
-        <v>0.48870582503369758</v>
+        <v>0.74379670380513963</v>
       </c>
       <c r="I182">
         <v>0</v>
@@ -9567,18 +9569,18 @@
         <v>0</v>
       </c>
       <c r="O182">
-        <v>1.0103885507437727</v>
+        <v>1.9422793832149141</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B183">
-        <v>28.753646018813022</v>
+        <v>22.41298740226209</v>
       </c>
       <c r="C183">
-        <v>0.26638251944622743</v>
+        <v>2.4343643720729444</v>
       </c>
       <c r="D183">
         <v>0</v>
@@ -9593,39 +9595,39 @@
         <v>0</v>
       </c>
       <c r="H183">
-        <v>0.74379670380513963</v>
+        <v>1.2847232941500739</v>
       </c>
       <c r="I183">
         <v>0</v>
       </c>
       <c r="J183">
-        <v>0</v>
+        <v>0.13139754741925555</v>
       </c>
       <c r="K183">
-        <v>0</v>
+        <v>0.12009656288557986</v>
       </c>
       <c r="L183">
         <v>0</v>
       </c>
       <c r="M183">
-        <v>0</v>
+        <v>6.3021792900221557E-2</v>
       </c>
       <c r="N183">
         <v>0</v>
       </c>
       <c r="O183">
-        <v>1.9422793832149141</v>
+        <v>3.8164516610272159</v>
       </c>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B184">
-        <v>22.41298740226209</v>
+        <v>53.010937290234956</v>
       </c>
       <c r="C184">
-        <v>2.4343643720729444</v>
+        <v>2.2158903285670415</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -9640,39 +9642,39 @@
         <v>0</v>
       </c>
       <c r="H184">
-        <v>1.2847232941500739</v>
+        <v>1.0403520318772559</v>
       </c>
       <c r="I184">
-        <v>0</v>
+        <v>3.627948667444101E-2</v>
       </c>
       <c r="J184">
-        <v>0.13139754741925555</v>
+        <v>0.15182150415655774</v>
       </c>
       <c r="K184">
-        <v>0.12009656288557986</v>
+        <v>6.7148749867230462E-2</v>
       </c>
       <c r="L184">
         <v>0</v>
       </c>
       <c r="M184">
-        <v>6.3021792900221557E-2</v>
+        <v>8.4644147124556646E-2</v>
       </c>
       <c r="N184">
         <v>0</v>
       </c>
       <c r="O184">
-        <v>3.8164516610272159</v>
+        <v>3.9405828508351712</v>
       </c>
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B185">
-        <v>53.010937290234956</v>
+        <v>49.96808204821275</v>
       </c>
       <c r="C185">
-        <v>2.2158903285670415</v>
+        <v>2.7414624641218666</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -9687,39 +9689,39 @@
         <v>0</v>
       </c>
       <c r="H185">
-        <v>1.0403520318772559</v>
+        <v>1.5115449770283393</v>
       </c>
       <c r="I185">
-        <v>3.627948667444101E-2</v>
+        <v>0.19532612254220363</v>
       </c>
       <c r="J185">
-        <v>0.15182150415655774</v>
+        <v>0.18825254469307492</v>
       </c>
       <c r="K185">
-        <v>6.7148749867230462E-2</v>
+        <v>0.12049851899967801</v>
       </c>
       <c r="L185">
         <v>0</v>
       </c>
       <c r="M185">
-        <v>8.4644147124556646E-2</v>
+        <v>0.22782175671685601</v>
       </c>
       <c r="N185">
         <v>0</v>
       </c>
       <c r="O185">
-        <v>3.9405828508351712</v>
+        <v>4.8791799471685291</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B186">
-        <v>49.96808204821275</v>
+        <v>46.21755826388241</v>
       </c>
       <c r="C186">
-        <v>2.7414624641218666</v>
+        <v>1.8551334779896211</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -9734,39 +9736,39 @@
         <v>0</v>
       </c>
       <c r="H186">
-        <v>1.5115449770283393</v>
+        <v>2.0743997343479981</v>
       </c>
       <c r="I186">
-        <v>0.19532612254220363</v>
+        <v>0.35315276067282059</v>
       </c>
       <c r="J186">
-        <v>0.18825254469307492</v>
+        <v>0.22087448275496138</v>
       </c>
       <c r="K186">
-        <v>0.12049851899967801</v>
+        <v>0.18742098038980617</v>
       </c>
       <c r="L186">
         <v>0</v>
       </c>
       <c r="M186">
-        <v>0.22782175671685601</v>
+        <v>0.46011136548279569</v>
       </c>
       <c r="N186">
         <v>0</v>
       </c>
       <c r="O186">
-        <v>4.8791799471685291</v>
+        <v>4.1540560350051585</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B187">
-        <v>46.21755826388241</v>
+        <v>47.246995193818996</v>
       </c>
       <c r="C187">
-        <v>1.8551334779896211</v>
+        <v>1.2374284729159515</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -9781,39 +9783,39 @@
         <v>0</v>
       </c>
       <c r="H187">
-        <v>2.0743997343479981</v>
+        <v>2.2284017234491982</v>
       </c>
       <c r="I187">
-        <v>0.35315276067282059</v>
+        <v>0.56039000098141933</v>
       </c>
       <c r="J187">
-        <v>0.22087448275496138</v>
+        <v>0.31324000295360593</v>
       </c>
       <c r="K187">
-        <v>0.18742098038980617</v>
+        <v>0.21531220831355802</v>
       </c>
       <c r="L187">
-        <v>0</v>
+        <v>0.15620397198049468</v>
       </c>
       <c r="M187">
-        <v>0.46011136548279569</v>
+        <v>0.61828569032542791</v>
       </c>
       <c r="N187">
         <v>0</v>
       </c>
       <c r="O187">
-        <v>4.1540560350051585</v>
+        <v>3.6847759895374477</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B188">
-        <v>47.246995193818996</v>
+        <v>0</v>
       </c>
       <c r="C188">
-        <v>1.2374284729159515</v>
+        <v>0</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -9828,33 +9830,33 @@
         <v>0</v>
       </c>
       <c r="H188">
-        <v>2.2284017234491982</v>
+        <v>0</v>
       </c>
       <c r="I188">
-        <v>0.56039000098141933</v>
+        <v>0</v>
       </c>
       <c r="J188">
-        <v>0.31324000295360593</v>
+        <v>0</v>
       </c>
       <c r="K188">
-        <v>0.21531220831355802</v>
+        <v>0</v>
       </c>
       <c r="L188">
-        <v>0.15620397198049468</v>
+        <v>0</v>
       </c>
       <c r="M188">
-        <v>0.61828569032542791</v>
+        <v>0</v>
       </c>
       <c r="N188">
         <v>0</v>
       </c>
       <c r="O188">
-        <v>3.6847759895374477</v>
+        <v>0.17261101503271992</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -9896,15 +9898,15 @@
         <v>0</v>
       </c>
       <c r="O189">
-        <v>0.17261101503271992</v>
+        <v>0.28971753169968123</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B190">
-        <v>0</v>
+        <v>31.472726540678195</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -9943,18 +9945,18 @@
         <v>0</v>
       </c>
       <c r="O190">
-        <v>0.28971753169968123</v>
+        <v>0.43997864396026309</v>
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B191">
-        <v>31.472726540678195</v>
+        <v>32.25118928408196</v>
       </c>
       <c r="C191">
-        <v>0</v>
+        <v>2.0277086977635552E-2</v>
       </c>
       <c r="D191">
         <v>0</v>
@@ -9969,7 +9971,7 @@
         <v>0</v>
       </c>
       <c r="H191">
-        <v>0</v>
+        <v>0.36288008448910852</v>
       </c>
       <c r="I191">
         <v>0</v>
@@ -9990,18 +9992,18 @@
         <v>0</v>
       </c>
       <c r="O191">
-        <v>0.43997864396026309</v>
+        <v>0.88152069682362999</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B192">
-        <v>32.25118928408196</v>
+        <v>28.897091935211968</v>
       </c>
       <c r="C192">
-        <v>2.0277086977635552E-2</v>
+        <v>0.12955086023569301</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -10016,7 +10018,7 @@
         <v>0</v>
       </c>
       <c r="H192">
-        <v>0.36288008448910852</v>
+        <v>0.59183780368507899</v>
       </c>
       <c r="I192">
         <v>0</v>
@@ -10037,18 +10039,18 @@
         <v>0</v>
       </c>
       <c r="O192">
-        <v>0.88152069682362999</v>
+        <v>1.6045460155334743</v>
       </c>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B193">
-        <v>28.897091935211968</v>
+        <v>24.385675999767052</v>
       </c>
       <c r="C193">
-        <v>0.12955086023569301</v>
+        <v>0.32957914704435542</v>
       </c>
       <c r="D193">
         <v>0</v>
@@ -10063,7 +10065,7 @@
         <v>0</v>
       </c>
       <c r="H193">
-        <v>0.59183780368507899</v>
+        <v>0.91306520098004151</v>
       </c>
       <c r="I193">
         <v>0</v>
@@ -10084,18 +10086,18 @@
         <v>0</v>
       </c>
       <c r="O193">
-        <v>1.6045460155334743</v>
+        <v>2.7482141935452558</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B194">
-        <v>24.385675999767052</v>
+        <v>20.154225663343905</v>
       </c>
       <c r="C194">
-        <v>0.32957914704435542</v>
+        <v>2.2009329928796837</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -10110,39 +10112,39 @@
         <v>0</v>
       </c>
       <c r="H194">
-        <v>0.91306520098004151</v>
+        <v>0.99871667878189552</v>
       </c>
       <c r="I194">
         <v>0</v>
       </c>
       <c r="J194">
-        <v>0</v>
+        <v>0.18023289885861621</v>
       </c>
       <c r="K194">
-        <v>0</v>
+        <v>0.11059826005601686</v>
       </c>
       <c r="L194">
         <v>0</v>
       </c>
       <c r="M194">
-        <v>0</v>
+        <v>0.1153712820957727</v>
       </c>
       <c r="N194">
         <v>0</v>
       </c>
       <c r="O194">
-        <v>2.7482141935452558</v>
+        <v>3.8226896167542002</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B195">
-        <v>20.154225663343905</v>
+        <v>55.871054477305634</v>
       </c>
       <c r="C195">
-        <v>2.2009329928796837</v>
+        <v>2.2892079472910725</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -10157,39 +10159,39 @@
         <v>0</v>
       </c>
       <c r="H195">
-        <v>0.99871667878189552</v>
+        <v>1.1771465431440027</v>
       </c>
       <c r="I195">
-        <v>0</v>
+        <v>5.2857323993215521E-2</v>
       </c>
       <c r="J195">
-        <v>0.18023289885861621</v>
+        <v>0.19105532429335412</v>
       </c>
       <c r="K195">
-        <v>0.11059826005601686</v>
+        <v>0.10914556053477255</v>
       </c>
       <c r="L195">
         <v>0</v>
       </c>
       <c r="M195">
-        <v>0.1153712820957727</v>
+        <v>7.9577475710236087E-2</v>
       </c>
       <c r="N195">
         <v>0</v>
       </c>
       <c r="O195">
-        <v>3.8226896167542002</v>
+        <v>3.8459377758916378</v>
       </c>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B196">
-        <v>55.871054477305634</v>
+        <v>43.816543767660242</v>
       </c>
       <c r="C196">
-        <v>2.2892079472910725</v>
+        <v>2.9758908519384231</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -10204,39 +10206,39 @@
         <v>0</v>
       </c>
       <c r="H196">
-        <v>1.1771465431440027</v>
+        <v>1.3509713570173101</v>
       </c>
       <c r="I196">
-        <v>5.2857323993215521E-2</v>
+        <v>0.20697361160318489</v>
       </c>
       <c r="J196">
-        <v>0.19105532429335412</v>
+        <v>0.28727032601998298</v>
       </c>
       <c r="K196">
-        <v>0.10914556053477255</v>
+        <v>0.20538777577806824</v>
       </c>
       <c r="L196">
-        <v>0</v>
+        <v>0.21104183805035456</v>
       </c>
       <c r="M196">
-        <v>7.9577475710236087E-2</v>
+        <v>0.26649519386978227</v>
       </c>
       <c r="N196">
         <v>0</v>
       </c>
       <c r="O196">
-        <v>3.8459377758916378</v>
+        <v>3.8759988120263404</v>
       </c>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B197">
-        <v>43.816543767660242</v>
+        <v>45.630878852307454</v>
       </c>
       <c r="C197">
-        <v>2.9758908519384231</v>
+        <v>2.8920319519955546</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -10251,39 +10253,39 @@
         <v>0</v>
       </c>
       <c r="H197">
-        <v>1.3509713570173101</v>
+        <v>1.9662366016695687</v>
       </c>
       <c r="I197">
-        <v>0.20697361160318489</v>
+        <v>0.37234550549106332</v>
       </c>
       <c r="J197">
-        <v>0.28727032601998298</v>
+        <v>0.51338679852554636</v>
       </c>
       <c r="K197">
-        <v>0.20538777577806824</v>
+        <v>0.26252518074207654</v>
       </c>
       <c r="L197">
-        <v>0.21104183805035456</v>
+        <v>0.31115991053930031</v>
       </c>
       <c r="M197">
-        <v>0.26649519386978227</v>
+        <v>0.67559057446953263</v>
       </c>
       <c r="N197">
         <v>0</v>
       </c>
       <c r="O197">
-        <v>3.8759988120263404</v>
+        <v>4.309191727635227</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B198">
-        <v>45.630878852307454</v>
+        <v>47.988593521116535</v>
       </c>
       <c r="C198">
-        <v>2.8920319519955546</v>
+        <v>1.7356245141872702</v>
       </c>
       <c r="D198">
         <v>0</v>
@@ -10298,39 +10300,39 @@
         <v>0</v>
       </c>
       <c r="H198">
-        <v>1.9662366016695687</v>
+        <v>2.4592158224115721</v>
       </c>
       <c r="I198">
-        <v>0.37234550549106332</v>
+        <v>0.42606201804089017</v>
       </c>
       <c r="J198">
-        <v>0.51338679852554636</v>
+        <v>0.53260454256173861</v>
       </c>
       <c r="K198">
-        <v>0.26252518074207654</v>
+        <v>0.33025627131012353</v>
       </c>
       <c r="L198">
-        <v>0.31115991053930031</v>
+        <v>0.4767965521286498</v>
       </c>
       <c r="M198">
-        <v>0.67559057446953263</v>
+        <v>0.84683499811355145</v>
       </c>
       <c r="N198">
         <v>0</v>
       </c>
       <c r="O198">
-        <v>4.309191727635227</v>
+        <v>3.7634164215770829</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B199">
-        <v>47.988593521116535</v>
+        <v>0</v>
       </c>
       <c r="C199">
-        <v>1.7356245141872702</v>
+        <v>0</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -10345,33 +10347,33 @@
         <v>0</v>
       </c>
       <c r="H199">
-        <v>2.4592158224115721</v>
+        <v>0</v>
       </c>
       <c r="I199">
-        <v>0.42606201804089017</v>
+        <v>0</v>
       </c>
       <c r="J199">
-        <v>0.53260454256173861</v>
+        <v>0</v>
       </c>
       <c r="K199">
-        <v>0.33025627131012353</v>
+        <v>0</v>
       </c>
       <c r="L199">
-        <v>0.4767965521286498</v>
+        <v>0</v>
       </c>
       <c r="M199">
-        <v>0.84683499811355145</v>
+        <v>0</v>
       </c>
       <c r="N199">
         <v>0</v>
       </c>
       <c r="O199">
-        <v>3.7634164215770829</v>
+        <v>0.18912118656579155</v>
       </c>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -10413,15 +10415,15 @@
         <v>0</v>
       </c>
       <c r="O200">
-        <v>0.18912118656579155</v>
+        <v>0.3016162993495049</v>
       </c>
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B201">
-        <v>0</v>
+        <v>30.71722205423734</v>
       </c>
       <c r="C201">
         <v>0</v>
@@ -10460,18 +10462,18 @@
         <v>0</v>
       </c>
       <c r="O201">
-        <v>0.3016162993495049</v>
+        <v>0.5922641009594678</v>
       </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B202">
-        <v>30.71722205423734</v>
+        <v>28.073410006153523</v>
       </c>
       <c r="C202">
-        <v>0</v>
+        <v>3.0803275535077113E-2</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -10486,7 +10488,7 @@
         <v>0</v>
       </c>
       <c r="H202">
-        <v>0</v>
+        <v>0.41926266621775354</v>
       </c>
       <c r="I202">
         <v>0</v>
@@ -10507,18 +10509,18 @@
         <v>0</v>
       </c>
       <c r="O202">
-        <v>0.5922641009594678</v>
+        <v>1.1816937731692321</v>
       </c>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B203">
-        <v>28.073410006153523</v>
+        <v>26.381952311914045</v>
       </c>
       <c r="C203">
-        <v>3.0803275535077113E-2</v>
+        <v>0.18953931778532318</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -10533,7 +10535,7 @@
         <v>0</v>
       </c>
       <c r="H203">
-        <v>0.41926266621775354</v>
+        <v>0.66511866970724265</v>
       </c>
       <c r="I203">
         <v>0</v>
@@ -10554,18 +10556,18 @@
         <v>0</v>
       </c>
       <c r="O203">
-        <v>1.1816937731692321</v>
+        <v>2.0753642015315914</v>
       </c>
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B204">
-        <v>26.381952311914045</v>
+        <v>25.045296948273563</v>
       </c>
       <c r="C204">
-        <v>0.18953931778532318</v>
+        <v>0.43940395617208799</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -10580,13 +10582,13 @@
         <v>0</v>
       </c>
       <c r="H204">
-        <v>0.66511866970724265</v>
+        <v>0.91293844493479281</v>
       </c>
       <c r="I204">
         <v>0</v>
       </c>
       <c r="J204">
-        <v>0</v>
+        <v>0.11202242405095937</v>
       </c>
       <c r="K204">
         <v>0</v>
@@ -10601,18 +10603,18 @@
         <v>0</v>
       </c>
       <c r="O204">
-        <v>2.0753642015315914</v>
+        <v>3.4673153872867575</v>
       </c>
     </row>
     <row r="205" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B205">
-        <v>25.045296948273563</v>
+        <v>21.762418838575016</v>
       </c>
       <c r="C205">
-        <v>0.43940395617208799</v>
+        <v>1.2233611120423036</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -10627,39 +10629,39 @@
         <v>0</v>
       </c>
       <c r="H205">
-        <v>0.91293844493479281</v>
+        <v>1.214030853467944</v>
       </c>
       <c r="I205">
         <v>0</v>
       </c>
       <c r="J205">
-        <v>0.11202242405095937</v>
+        <v>0.10424138322565431</v>
       </c>
       <c r="K205">
-        <v>0</v>
+        <v>0.22817472397633792</v>
       </c>
       <c r="L205">
-        <v>0</v>
+        <v>0.20567206691260745</v>
       </c>
       <c r="M205">
-        <v>0</v>
+        <v>8.4189473276039331E-2</v>
       </c>
       <c r="N205">
         <v>0</v>
       </c>
       <c r="O205">
-        <v>3.4673153872867575</v>
+        <v>4.5693894288319381</v>
       </c>
     </row>
     <row r="206" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B206">
-        <v>21.762418838575016</v>
+        <v>56.33283154570185</v>
       </c>
       <c r="C206">
-        <v>1.2233611120423036</v>
+        <v>1.3553468317047028</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -10674,39 +10676,39 @@
         <v>0</v>
       </c>
       <c r="H206">
-        <v>1.214030853467944</v>
+        <v>1.101350214213054</v>
       </c>
       <c r="I206">
-        <v>0</v>
+        <v>4.2087376212465673E-2</v>
       </c>
       <c r="J206">
-        <v>0.10424138322565431</v>
+        <v>0.32505542545760785</v>
       </c>
       <c r="K206">
-        <v>0.22817472397633792</v>
+        <v>0.13721191055932067</v>
       </c>
       <c r="L206">
-        <v>0.20567206691260745</v>
+        <v>0.21879276888309881</v>
       </c>
       <c r="M206">
-        <v>8.4189473276039331E-2</v>
+        <v>0</v>
       </c>
       <c r="N206">
         <v>0</v>
       </c>
       <c r="O206">
-        <v>4.5693894288319381</v>
+        <v>4.366179617970336</v>
       </c>
     </row>
     <row r="207" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B207">
-        <v>56.33283154570185</v>
+        <v>48.916254618077204</v>
       </c>
       <c r="C207">
-        <v>1.3553468317047028</v>
+        <v>1.2737925974662152</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -10721,39 +10723,39 @@
         <v>0</v>
       </c>
       <c r="H207">
-        <v>1.101350214213054</v>
+        <v>1.2043134272409395</v>
       </c>
       <c r="I207">
-        <v>4.2087376212465673E-2</v>
+        <v>0.16195263216014352</v>
       </c>
       <c r="J207">
-        <v>0.32505542545760785</v>
+        <v>0.39219481207733198</v>
       </c>
       <c r="K207">
-        <v>0.13721191055932067</v>
+        <v>0.3009883711507868</v>
       </c>
       <c r="L207">
-        <v>0.21879276888309881</v>
+        <v>0.44396369146214665</v>
       </c>
       <c r="M207">
-        <v>0</v>
+        <v>0.19471997334958671</v>
       </c>
       <c r="N207">
         <v>0</v>
       </c>
       <c r="O207">
-        <v>4.366179617970336</v>
+        <v>4.522060750442594</v>
       </c>
     </row>
     <row r="208" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B208">
-        <v>48.916254618077204</v>
+        <v>52.28496147586813</v>
       </c>
       <c r="C208">
-        <v>1.2737925974662152</v>
+        <v>0.71854627416972372</v>
       </c>
       <c r="D208">
         <v>0</v>
@@ -10768,39 +10770,39 @@
         <v>0</v>
       </c>
       <c r="H208">
-        <v>1.2043134272409395</v>
+        <v>1.2998182287158897</v>
       </c>
       <c r="I208">
-        <v>0.16195263216014352</v>
+        <v>0.26729175023664231</v>
       </c>
       <c r="J208">
-        <v>0.39219481207733198</v>
+        <v>0.44931189297059793</v>
       </c>
       <c r="K208">
-        <v>0.3009883711507868</v>
+        <v>0.3959185423599948</v>
       </c>
       <c r="L208">
-        <v>0.44396369146214665</v>
+        <v>0.89179514276963046</v>
       </c>
       <c r="M208">
-        <v>0.19471997334958671</v>
+        <v>0.43046814723809879</v>
       </c>
       <c r="N208">
         <v>0</v>
       </c>
       <c r="O208">
-        <v>4.522060750442594</v>
+        <v>3.9445052514132342</v>
       </c>
     </row>
     <row r="209" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B209">
-        <v>52.28496147586813</v>
+        <v>48.814065435851816</v>
       </c>
       <c r="C209">
-        <v>0.71854627416972372</v>
+        <v>0.37730400981341072</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -10815,79 +10817,33 @@
         <v>0</v>
       </c>
       <c r="H209">
-        <v>1.2998182287158897</v>
+        <v>1.3686017082429383</v>
       </c>
       <c r="I209">
-        <v>0.26729175023664231</v>
+        <v>0.24591115913729458</v>
       </c>
       <c r="J209">
-        <v>0.44931189297059793</v>
+        <v>0.50770737080541706</v>
       </c>
       <c r="K209">
-        <v>0.3959185423599948</v>
+        <v>0.51635186646277198</v>
       </c>
       <c r="L209">
-        <v>0.89179514276963046</v>
+        <v>0.86574385461561854</v>
       </c>
       <c r="M209">
-        <v>0.43046814723809879</v>
+        <v>0.91745650805223644</v>
       </c>
       <c r="N209">
         <v>0</v>
       </c>
       <c r="O209">
-        <v>3.9445052514132342</v>
-      </c>
-    </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A210" t="s">
-        <v>222</v>
-      </c>
-      <c r="B210">
-        <v>48.814065435851816</v>
-      </c>
-      <c r="C210">
-        <v>0.37730400981341072</v>
-      </c>
-      <c r="D210">
-        <v>0</v>
-      </c>
-      <c r="E210">
-        <v>0</v>
-      </c>
-      <c r="F210">
-        <v>0</v>
-      </c>
-      <c r="G210">
-        <v>0</v>
-      </c>
-      <c r="H210">
-        <v>1.3686017082429383</v>
-      </c>
-      <c r="I210">
-        <v>0.24591115913729458</v>
-      </c>
-      <c r="J210">
-        <v>0.50770737080541706</v>
-      </c>
-      <c r="K210">
-        <v>0.51635186646277198</v>
-      </c>
-      <c r="L210">
-        <v>0.86574385461561854</v>
-      </c>
-      <c r="M210">
-        <v>0.91745650805223644</v>
-      </c>
-      <c r="N210">
-        <v>0</v>
-      </c>
-      <c r="O210">
         <v>4.3433607179449378</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Removed duplicate row from sample data
</commit_message>
<xml_diff>
--- a/tests/sample_input_data.xlsx
+++ b/tests/sample_input_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="223">
   <si>
     <t>OD600</t>
   </si>
@@ -1011,20 +1011,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O209"/>
+  <dimension ref="A1:O208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="J207" sqref="J207"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A167" sqref="A167:XFD167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>6.3904438957407966E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>0.13519519413948108</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>0.36159329512181815</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>1.2556213135593297</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>3.1066495911097651</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>3.3257900484150862</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>9.737728692032098</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>10.100702295851852</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>8.6666916758756738</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>7.6375775548227942</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>9.9104581447884232</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>10.472626332886657</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>7.2958975597312845</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>7.0525095741553259E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>0.12840497486193755</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>0.39782447459024162</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>1.3087621885422489</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>2.8189313671752334</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>4.4602806230617222</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>9.6438614091511123</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>9.971647468383086</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>7.6452640582975953</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>8.2846753465561171</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>8.1801174797830161</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>8.7487077692298261</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>6.3310442171037984</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>0.212150197491316</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>0.38515544443496058</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>1.189400586260829</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>3.7783059584606269</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>10.560979361086696</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>9.770597056946265</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>10.341521706181071</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>8.4639584513798862</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>7.3952397464694348</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>7.0149340095844339</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>10.020034161676389</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>10.790349666986497</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>0.19864688711037753</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>0.39271616828316308</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>1.0867830631467963</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>3.7142199541180179</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>10.283860084517867</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>11.179723473196304</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>11.023780984800251</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>9.6595831660487779</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>7.1011406321415791</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>7.0667337758922262</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>8.5707063200991431</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>12.644291283460488</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>0.20640832551642807</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>0.44421587928103057</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>1.1886154087645457</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>3.7572949788945298</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>12.83077780644388</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>72</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>9.3285491179877127</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>73</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>9.3123173085057633</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>7.9408759517748013</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>8.0696539447389561</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>7.5975833260018808</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>8.5221347418901292</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>9.2480517097766857</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>132</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>0.20435875996200512</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>0.57476748118036125</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>1.657261514319663</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>5.3057243551108701</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>11.327170529469193</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>137</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>8.4431035477391507</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>8.6890933338379188</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>139</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>8.7216519859264068</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>140</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>7.3788328487715233</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>141</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>6.9763077043884767</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>142</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>10.078843077835428</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>143</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>9.4656481381500601</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>144</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>0.21243300069594007</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>145</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>0.62085582545595774</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>146</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>2.2133843951639345</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>5.7842599271121129</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>148</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>14.015325923099077</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>149</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>8.1432212448837547</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>150</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>8.4164787906316612</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>151</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>8.7471827897025793</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>152</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>8.579253339642122</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>153</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>6.6211275515430517</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>154</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>9.1498000016872663</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>155</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>8.9982179444296353</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>156</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>0.21815586818091748</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>157</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>0.5518044459865783</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>158</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>1.9866014157919967</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>159</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>6.2191168133923105</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>160</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>11.601180950078289</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>161</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>10.195778792819718</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>162</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>8.9938611984996388</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>163</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>7.1204930700394415</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>164</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>9.0866608013220187</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>165</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>8.0024050591427187</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>166</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>9.2360510611180135</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>167</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>9.539845080146975</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>79</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>0.16729763737852874</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>80</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>0.28928098069453828</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>81</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>0.84555104955919436</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>82</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>1.8237090697615967</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>83</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>4.1734205290874389</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>84</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>8.1559990684671941</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>85</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>9.1776551606997714</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>86</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>8.8749204578435137</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>87</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>7.1887741720082694</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>88</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>8.1282970644593178</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>89</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>8.5272212724377301</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>90</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>0.14748818726989976</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>91</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>0.31181116730123565</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>92</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>0.68244029911544235</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>93</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>1.8911056078268749</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>94</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>3.5539459603685191</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>95</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>6.5924840424200557</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>96</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>7.660607035645187</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>97</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>8.2587401637936502</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>98</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>7.0256104818385179</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>99</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>7.4411273816854964</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>100</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>6.747873305270744</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>101</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>0.17686683345236009</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>102</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>0.30452097426355823</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>103</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>0.73366971471484999</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>104</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>1.8637769070624877</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>105</v>
       </c>
@@ -6987,7 +6987,7 @@
         <v>4.1166025478456207</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>106</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>7.3736806615012496</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>107</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>8.9766280063950852</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>108</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>8.0669061631012227</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>109</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>7.4714632555891232</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>110</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>8.1999468012489096</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>111</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>8.3847393933964494</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>168</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>0.18808368748784937</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>169</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>0.29800403481393373</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>170</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>0.73119583237324459</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>171</v>
       </c>
@@ -7457,7 +7457,7 @@
         <v>1.9120437622348265</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>172</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>4.6495455663710965</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>173</v>
       </c>
@@ -7551,7 +7551,7 @@
         <v>7.8078847255551214</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>174</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>8.8027679194022141</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>175</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>7.7288720925261005</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>176</v>
       </c>
@@ -7692,7 +7692,7 @@
         <v>9.1150698639150693</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>177</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>8.8842683961937681</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>178</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>8.8895858252579902</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>179</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>0.19638050808511945</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>180</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>0.29384820916441373</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>181</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>0.74104333309649828</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>182</v>
       </c>
@@ -7974,7 +7974,7 @@
         <v>2.070194021123827</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>183</v>
       </c>
@@ -8021,7 +8021,7 @@
         <v>5.3121206773495446</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>184</v>
       </c>
@@ -8068,7 +8068,7 @@
         <v>7.8588139710176703</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>185</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>9.8892371030759865</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>186</v>
       </c>
@@ -8162,7 +8162,7 @@
         <v>9.2002030466200306</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>187</v>
       </c>
@@ -8209,7 +8209,7 @@
         <v>9.875374076264384</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>188</v>
       </c>
@@ -8256,7 +8256,7 @@
         <v>10.027415902071036</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>189</v>
       </c>
@@ -8303,7 +8303,7 @@
         <v>9.9689379649155203</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>112</v>
       </c>
@@ -8350,7 +8350,7 @@
         <v>0.24271500306581498</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>113</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>0.45999899419884321</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>114</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>0.92715936065265681</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>115</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>1.6885900555849649</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>116</v>
       </c>
@@ -8538,7 +8538,7 @@
         <v>3.2453715503303222</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>117</v>
       </c>
@@ -8585,7 +8585,7 @@
         <v>5.3771826439194639</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>118</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>5.3391426026155697</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>119</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>5.2184680356032844</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>120</v>
       </c>
@@ -8726,7 +8726,7 @@
         <v>4.4579247848171839</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>121</v>
       </c>
@@ -8773,7 +8773,7 @@
         <v>4.3770611569154791</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>122</v>
       </c>
@@ -8820,12 +8820,12 @@
         <v>0.19839558540886784</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B167">
-        <v>0</v>
+        <v>26.210711440416187</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -8849,7 +8849,7 @@
         <v>0</v>
       </c>
       <c r="J167">
-        <v>0</v>
+        <v>2.2828721062786262E-2</v>
       </c>
       <c r="K167">
         <v>0</v>
@@ -8864,18 +8864,18 @@
         <v>0</v>
       </c>
       <c r="O167">
-        <v>0.28816926804258314</v>
-      </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.50879774293282409</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B168">
-        <v>26.210711440416187</v>
+        <v>30.488156600878433</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>2.8689321614988109E-2</v>
       </c>
       <c r="D168">
         <v>0</v>
@@ -8890,13 +8890,13 @@
         <v>0</v>
       </c>
       <c r="H168">
-        <v>0</v>
+        <v>0.43122666288151518</v>
       </c>
       <c r="I168">
         <v>0</v>
       </c>
       <c r="J168">
-        <v>2.2828721062786262E-2</v>
+        <v>0.15478889768656159</v>
       </c>
       <c r="K168">
         <v>0</v>
@@ -8911,18 +8911,18 @@
         <v>0</v>
       </c>
       <c r="O168">
-        <v>0.50879774293282409</v>
-      </c>
-    </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1.264799702961529</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B169">
-        <v>30.488156600878433</v>
+        <v>27.166575315254747</v>
       </c>
       <c r="C169">
-        <v>2.8689321614988109E-2</v>
+        <v>5.6610460511909183E-2</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -8937,39 +8937,39 @@
         <v>0</v>
       </c>
       <c r="H169">
-        <v>0.43122666288151518</v>
+        <v>0.57646630540589217</v>
       </c>
       <c r="I169">
         <v>0</v>
       </c>
       <c r="J169">
-        <v>0.15478889768656159</v>
+        <v>0.23777615957797937</v>
       </c>
       <c r="K169">
-        <v>0</v>
+        <v>3.2079268871719364E-2</v>
       </c>
       <c r="L169">
         <v>0</v>
       </c>
       <c r="M169">
-        <v>0</v>
+        <v>5.2654594269875191E-2</v>
       </c>
       <c r="N169">
         <v>0</v>
       </c>
       <c r="O169">
-        <v>1.264799702961529</v>
-      </c>
-    </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.45">
+        <v>2.3560223866467136</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B170">
-        <v>27.166575315254747</v>
+        <v>24.785949276769905</v>
       </c>
       <c r="C170">
-        <v>5.6610460511909183E-2</v>
+        <v>0.15703367867823609</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -8984,39 +8984,39 @@
         <v>0</v>
       </c>
       <c r="H170">
-        <v>0.57646630540589217</v>
+        <v>0.84470930262009747</v>
       </c>
       <c r="I170">
         <v>0</v>
       </c>
       <c r="J170">
-        <v>0.23777615957797937</v>
+        <v>0.13526230526909322</v>
       </c>
       <c r="K170">
-        <v>3.2079268871719364E-2</v>
+        <v>9.8090908726610471E-2</v>
       </c>
       <c r="L170">
         <v>0</v>
       </c>
       <c r="M170">
-        <v>5.2654594269875191E-2</v>
+        <v>0.11901854856539847</v>
       </c>
       <c r="N170">
         <v>0</v>
       </c>
       <c r="O170">
-        <v>2.3560223866467136</v>
-      </c>
-    </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4.0108155464101882</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B171">
-        <v>24.785949276769905</v>
+        <v>14.020345630622408</v>
       </c>
       <c r="C171">
-        <v>0.15703367867823609</v>
+        <v>0.18338333956402442</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -9031,39 +9031,39 @@
         <v>0</v>
       </c>
       <c r="H171">
-        <v>0.84470930262009747</v>
+        <v>0.86937005453584748</v>
       </c>
       <c r="I171">
-        <v>0</v>
+        <v>0.23818354381210421</v>
       </c>
       <c r="J171">
-        <v>0.13526230526909322</v>
+        <v>0.77063603233654498</v>
       </c>
       <c r="K171">
-        <v>9.8090908726610471E-2</v>
+        <v>0.4928697060431429</v>
       </c>
       <c r="L171">
-        <v>0</v>
+        <v>0.64416526185391954</v>
       </c>
       <c r="M171">
-        <v>0.11901854856539847</v>
+        <v>0.5069068947054588</v>
       </c>
       <c r="N171">
         <v>0</v>
       </c>
       <c r="O171">
-        <v>4.0108155464101882</v>
-      </c>
-    </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.45">
+        <v>6.0576031542629982</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B172">
-        <v>14.020345630622408</v>
+        <v>41.963513241641017</v>
       </c>
       <c r="C172">
-        <v>0.18338333956402442</v>
+        <v>0.20977635404843351</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -9078,39 +9078,39 @@
         <v>0</v>
       </c>
       <c r="H172">
-        <v>0.86937005453584748</v>
+        <v>0.74393685810075749</v>
       </c>
       <c r="I172">
-        <v>0.23818354381210421</v>
+        <v>0.22150348127025926</v>
       </c>
       <c r="J172">
-        <v>0.77063603233654498</v>
+        <v>0.72077960948721165</v>
       </c>
       <c r="K172">
-        <v>0.4928697060431429</v>
+        <v>0.45079457485114444</v>
       </c>
       <c r="L172">
-        <v>0.64416526185391954</v>
+        <v>0.62622872466825497</v>
       </c>
       <c r="M172">
-        <v>0.5069068947054588</v>
+        <v>0.52686595545976</v>
       </c>
       <c r="N172">
         <v>0</v>
       </c>
       <c r="O172">
-        <v>6.0576031542629982</v>
-      </c>
-    </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.45">
+        <v>5.7115012870102415</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B173">
-        <v>41.963513241641017</v>
+        <v>39.499278943357439</v>
       </c>
       <c r="C173">
-        <v>0.20977635404843351</v>
+        <v>2.1820076099513093E-2</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -9125,39 +9125,39 @@
         <v>0</v>
       </c>
       <c r="H173">
-        <v>0.74393685810075749</v>
+        <v>0.94208939986753792</v>
       </c>
       <c r="I173">
-        <v>0.22150348127025926</v>
+        <v>0.45025135263218713</v>
       </c>
       <c r="J173">
-        <v>0.72077960948721165</v>
+        <v>0.70218171636319726</v>
       </c>
       <c r="K173">
-        <v>0.45079457485114444</v>
+        <v>0.79743096556173865</v>
       </c>
       <c r="L173">
-        <v>0.62622872466825497</v>
+        <v>1.0808986028628471</v>
       </c>
       <c r="M173">
-        <v>0.52686595545976</v>
+        <v>0.88166297696335316</v>
       </c>
       <c r="N173">
         <v>0</v>
       </c>
       <c r="O173">
-        <v>5.7115012870102415</v>
-      </c>
-    </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.45">
+        <v>5.9502650635308214</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B174">
-        <v>39.499278943357439</v>
+        <v>35.691159213772508</v>
       </c>
       <c r="C174">
-        <v>2.1820076099513093E-2</v>
+        <v>0</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -9172,36 +9172,36 @@
         <v>0</v>
       </c>
       <c r="H174">
-        <v>0.94208939986753792</v>
+        <v>0.92179866292826851</v>
       </c>
       <c r="I174">
-        <v>0.45025135263218713</v>
+        <v>0.59413649814594571</v>
       </c>
       <c r="J174">
-        <v>0.70218171636319726</v>
+        <v>0.57995649991007026</v>
       </c>
       <c r="K174">
-        <v>0.79743096556173865</v>
+        <v>0.98469838109258723</v>
       </c>
       <c r="L174">
-        <v>1.0808986028628471</v>
+        <v>1.5691838706186596</v>
       </c>
       <c r="M174">
-        <v>0.88166297696335316</v>
+        <v>1.192902617256095</v>
       </c>
       <c r="N174">
         <v>0</v>
       </c>
       <c r="O174">
-        <v>5.9502650635308214</v>
-      </c>
-    </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.45">
+        <v>5.5225275359599904</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B175">
-        <v>35.691159213772508</v>
+        <v>39.262442284367303</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -9219,36 +9219,36 @@
         <v>0</v>
       </c>
       <c r="H175">
-        <v>0.92179866292826851</v>
+        <v>0.87485561878762985</v>
       </c>
       <c r="I175">
-        <v>0.59413649814594571</v>
+        <v>0.82810782726369692</v>
       </c>
       <c r="J175">
-        <v>0.57995649991007026</v>
+        <v>0.57024439837900442</v>
       </c>
       <c r="K175">
-        <v>0.98469838109258723</v>
+        <v>1.2762860100959026</v>
       </c>
       <c r="L175">
-        <v>1.5691838706186596</v>
+        <v>2.1067085510888228</v>
       </c>
       <c r="M175">
-        <v>1.192902617256095</v>
+        <v>1.5909530600597361</v>
       </c>
       <c r="N175">
         <v>0</v>
       </c>
       <c r="O175">
-        <v>5.5225275359599904</v>
-      </c>
-    </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4.8295154702838037</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>131</v>
+        <v>190</v>
       </c>
       <c r="B176">
-        <v>39.262442284367303</v>
+        <v>0</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -9266,33 +9266,33 @@
         <v>0</v>
       </c>
       <c r="H176">
-        <v>0.87485561878762985</v>
+        <v>0</v>
       </c>
       <c r="I176">
-        <v>0.82810782726369692</v>
+        <v>0</v>
       </c>
       <c r="J176">
-        <v>0.57024439837900442</v>
+        <v>0</v>
       </c>
       <c r="K176">
-        <v>1.2762860100959026</v>
+        <v>0</v>
       </c>
       <c r="L176">
-        <v>2.1067085510888228</v>
+        <v>0</v>
       </c>
       <c r="M176">
-        <v>1.5909530600597361</v>
+        <v>0</v>
       </c>
       <c r="N176">
         <v>0</v>
       </c>
       <c r="O176">
-        <v>4.8295154702838037</v>
-      </c>
-    </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.16602462016966377</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -9334,15 +9334,15 @@
         <v>0</v>
       </c>
       <c r="O177">
-        <v>0.16602462016966377</v>
-      </c>
-    </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.20677910561152099</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B178">
-        <v>0</v>
+        <v>32.616358749104343</v>
       </c>
       <c r="C178">
         <v>0</v>
@@ -9381,18 +9381,18 @@
         <v>0</v>
       </c>
       <c r="O178">
-        <v>0.20677910561152099</v>
-      </c>
-    </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.23527309636057306</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B179">
-        <v>32.616358749104343</v>
+        <v>31.792176921235782</v>
       </c>
       <c r="C179">
-        <v>0</v>
+        <v>1.410715185241304E-2</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -9407,7 +9407,7 @@
         <v>0</v>
       </c>
       <c r="H179">
-        <v>0</v>
+        <v>0.31836657709076677</v>
       </c>
       <c r="I179">
         <v>0</v>
@@ -9428,18 +9428,18 @@
         <v>0</v>
       </c>
       <c r="O179">
-        <v>0.23527309636057306</v>
-      </c>
-    </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.72329210403087296</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B180">
-        <v>31.792176921235782</v>
+        <v>30.471930695350832</v>
       </c>
       <c r="C180">
-        <v>1.410715185241304E-2</v>
+        <v>0.10427530425080749</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -9454,7 +9454,7 @@
         <v>0</v>
       </c>
       <c r="H180">
-        <v>0.31836657709076677</v>
+        <v>0.48870582503369758</v>
       </c>
       <c r="I180">
         <v>0</v>
@@ -9475,18 +9475,18 @@
         <v>0</v>
       </c>
       <c r="O180">
-        <v>0.72329210403087296</v>
-      </c>
-    </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1.0103885507437727</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B181">
-        <v>30.471930695350832</v>
+        <v>28.753646018813022</v>
       </c>
       <c r="C181">
-        <v>0.10427530425080749</v>
+        <v>0.26638251944622743</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -9501,7 +9501,7 @@
         <v>0</v>
       </c>
       <c r="H181">
-        <v>0.48870582503369758</v>
+        <v>0.74379670380513963</v>
       </c>
       <c r="I181">
         <v>0</v>
@@ -9522,18 +9522,18 @@
         <v>0</v>
       </c>
       <c r="O181">
-        <v>1.0103885507437727</v>
-      </c>
-    </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1.9422793832149141</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B182">
-        <v>28.753646018813022</v>
+        <v>22.41298740226209</v>
       </c>
       <c r="C182">
-        <v>0.26638251944622743</v>
+        <v>2.4343643720729444</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -9548,39 +9548,39 @@
         <v>0</v>
       </c>
       <c r="H182">
-        <v>0.74379670380513963</v>
+        <v>1.2847232941500739</v>
       </c>
       <c r="I182">
         <v>0</v>
       </c>
       <c r="J182">
-        <v>0</v>
+        <v>0.13139754741925555</v>
       </c>
       <c r="K182">
-        <v>0</v>
+        <v>0.12009656288557986</v>
       </c>
       <c r="L182">
         <v>0</v>
       </c>
       <c r="M182">
-        <v>0</v>
+        <v>6.3021792900221557E-2</v>
       </c>
       <c r="N182">
         <v>0</v>
       </c>
       <c r="O182">
-        <v>1.9422793832149141</v>
-      </c>
-    </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.8164516610272159</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B183">
-        <v>22.41298740226209</v>
+        <v>53.010937290234956</v>
       </c>
       <c r="C183">
-        <v>2.4343643720729444</v>
+        <v>2.2158903285670415</v>
       </c>
       <c r="D183">
         <v>0</v>
@@ -9595,39 +9595,39 @@
         <v>0</v>
       </c>
       <c r="H183">
-        <v>1.2847232941500739</v>
+        <v>1.0403520318772559</v>
       </c>
       <c r="I183">
-        <v>0</v>
+        <v>3.627948667444101E-2</v>
       </c>
       <c r="J183">
-        <v>0.13139754741925555</v>
+        <v>0.15182150415655774</v>
       </c>
       <c r="K183">
-        <v>0.12009656288557986</v>
+        <v>6.7148749867230462E-2</v>
       </c>
       <c r="L183">
         <v>0</v>
       </c>
       <c r="M183">
-        <v>6.3021792900221557E-2</v>
+        <v>8.4644147124556646E-2</v>
       </c>
       <c r="N183">
         <v>0</v>
       </c>
       <c r="O183">
-        <v>3.8164516610272159</v>
-      </c>
-    </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.9405828508351712</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B184">
-        <v>53.010937290234956</v>
+        <v>49.96808204821275</v>
       </c>
       <c r="C184">
-        <v>2.2158903285670415</v>
+        <v>2.7414624641218666</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -9642,39 +9642,39 @@
         <v>0</v>
       </c>
       <c r="H184">
-        <v>1.0403520318772559</v>
+        <v>1.5115449770283393</v>
       </c>
       <c r="I184">
-        <v>3.627948667444101E-2</v>
+        <v>0.19532612254220363</v>
       </c>
       <c r="J184">
-        <v>0.15182150415655774</v>
+        <v>0.18825254469307492</v>
       </c>
       <c r="K184">
-        <v>6.7148749867230462E-2</v>
+        <v>0.12049851899967801</v>
       </c>
       <c r="L184">
         <v>0</v>
       </c>
       <c r="M184">
-        <v>8.4644147124556646E-2</v>
+        <v>0.22782175671685601</v>
       </c>
       <c r="N184">
         <v>0</v>
       </c>
       <c r="O184">
-        <v>3.9405828508351712</v>
-      </c>
-    </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4.8791799471685291</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B185">
-        <v>49.96808204821275</v>
+        <v>46.21755826388241</v>
       </c>
       <c r="C185">
-        <v>2.7414624641218666</v>
+        <v>1.8551334779896211</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -9689,39 +9689,39 @@
         <v>0</v>
       </c>
       <c r="H185">
-        <v>1.5115449770283393</v>
+        <v>2.0743997343479981</v>
       </c>
       <c r="I185">
-        <v>0.19532612254220363</v>
+        <v>0.35315276067282059</v>
       </c>
       <c r="J185">
-        <v>0.18825254469307492</v>
+        <v>0.22087448275496138</v>
       </c>
       <c r="K185">
-        <v>0.12049851899967801</v>
+        <v>0.18742098038980617</v>
       </c>
       <c r="L185">
         <v>0</v>
       </c>
       <c r="M185">
-        <v>0.22782175671685601</v>
+        <v>0.46011136548279569</v>
       </c>
       <c r="N185">
         <v>0</v>
       </c>
       <c r="O185">
-        <v>4.8791799471685291</v>
-      </c>
-    </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4.1540560350051585</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B186">
-        <v>46.21755826388241</v>
+        <v>47.246995193818996</v>
       </c>
       <c r="C186">
-        <v>1.8551334779896211</v>
+        <v>1.2374284729159515</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -9736,39 +9736,39 @@
         <v>0</v>
       </c>
       <c r="H186">
-        <v>2.0743997343479981</v>
+        <v>2.2284017234491982</v>
       </c>
       <c r="I186">
-        <v>0.35315276067282059</v>
+        <v>0.56039000098141933</v>
       </c>
       <c r="J186">
-        <v>0.22087448275496138</v>
+        <v>0.31324000295360593</v>
       </c>
       <c r="K186">
-        <v>0.18742098038980617</v>
+        <v>0.21531220831355802</v>
       </c>
       <c r="L186">
-        <v>0</v>
+        <v>0.15620397198049468</v>
       </c>
       <c r="M186">
-        <v>0.46011136548279569</v>
+        <v>0.61828569032542791</v>
       </c>
       <c r="N186">
         <v>0</v>
       </c>
       <c r="O186">
-        <v>4.1540560350051585</v>
-      </c>
-    </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.6847759895374477</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B187">
-        <v>47.246995193818996</v>
+        <v>0</v>
       </c>
       <c r="C187">
-        <v>1.2374284729159515</v>
+        <v>0</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -9783,33 +9783,33 @@
         <v>0</v>
       </c>
       <c r="H187">
-        <v>2.2284017234491982</v>
+        <v>0</v>
       </c>
       <c r="I187">
-        <v>0.56039000098141933</v>
+        <v>0</v>
       </c>
       <c r="J187">
-        <v>0.31324000295360593</v>
+        <v>0</v>
       </c>
       <c r="K187">
-        <v>0.21531220831355802</v>
+        <v>0</v>
       </c>
       <c r="L187">
-        <v>0.15620397198049468</v>
+        <v>0</v>
       </c>
       <c r="M187">
-        <v>0.61828569032542791</v>
+        <v>0</v>
       </c>
       <c r="N187">
         <v>0</v>
       </c>
       <c r="O187">
-        <v>3.6847759895374477</v>
-      </c>
-    </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.17261101503271992</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -9851,15 +9851,15 @@
         <v>0</v>
       </c>
       <c r="O188">
-        <v>0.17261101503271992</v>
-      </c>
-    </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.28971753169968123</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B189">
-        <v>0</v>
+        <v>31.472726540678195</v>
       </c>
       <c r="C189">
         <v>0</v>
@@ -9898,18 +9898,18 @@
         <v>0</v>
       </c>
       <c r="O189">
-        <v>0.28971753169968123</v>
-      </c>
-    </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.43997864396026309</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B190">
-        <v>31.472726540678195</v>
+        <v>32.25118928408196</v>
       </c>
       <c r="C190">
-        <v>0</v>
+        <v>2.0277086977635552E-2</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -9924,7 +9924,7 @@
         <v>0</v>
       </c>
       <c r="H190">
-        <v>0</v>
+        <v>0.36288008448910852</v>
       </c>
       <c r="I190">
         <v>0</v>
@@ -9945,18 +9945,18 @@
         <v>0</v>
       </c>
       <c r="O190">
-        <v>0.43997864396026309</v>
-      </c>
-    </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.88152069682362999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B191">
-        <v>32.25118928408196</v>
+        <v>28.897091935211968</v>
       </c>
       <c r="C191">
-        <v>2.0277086977635552E-2</v>
+        <v>0.12955086023569301</v>
       </c>
       <c r="D191">
         <v>0</v>
@@ -9971,7 +9971,7 @@
         <v>0</v>
       </c>
       <c r="H191">
-        <v>0.36288008448910852</v>
+        <v>0.59183780368507899</v>
       </c>
       <c r="I191">
         <v>0</v>
@@ -9992,18 +9992,18 @@
         <v>0</v>
       </c>
       <c r="O191">
-        <v>0.88152069682362999</v>
-      </c>
-    </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1.6045460155334743</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B192">
-        <v>28.897091935211968</v>
+        <v>24.385675999767052</v>
       </c>
       <c r="C192">
-        <v>0.12955086023569301</v>
+        <v>0.32957914704435542</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -10018,7 +10018,7 @@
         <v>0</v>
       </c>
       <c r="H192">
-        <v>0.59183780368507899</v>
+        <v>0.91306520098004151</v>
       </c>
       <c r="I192">
         <v>0</v>
@@ -10039,18 +10039,18 @@
         <v>0</v>
       </c>
       <c r="O192">
-        <v>1.6045460155334743</v>
-      </c>
-    </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.45">
+        <v>2.7482141935452558</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B193">
-        <v>24.385675999767052</v>
+        <v>20.154225663343905</v>
       </c>
       <c r="C193">
-        <v>0.32957914704435542</v>
+        <v>2.2009329928796837</v>
       </c>
       <c r="D193">
         <v>0</v>
@@ -10065,39 +10065,39 @@
         <v>0</v>
       </c>
       <c r="H193">
-        <v>0.91306520098004151</v>
+        <v>0.99871667878189552</v>
       </c>
       <c r="I193">
         <v>0</v>
       </c>
       <c r="J193">
-        <v>0</v>
+        <v>0.18023289885861621</v>
       </c>
       <c r="K193">
-        <v>0</v>
+        <v>0.11059826005601686</v>
       </c>
       <c r="L193">
         <v>0</v>
       </c>
       <c r="M193">
-        <v>0</v>
+        <v>0.1153712820957727</v>
       </c>
       <c r="N193">
         <v>0</v>
       </c>
       <c r="O193">
-        <v>2.7482141935452558</v>
-      </c>
-    </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.8226896167542002</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B194">
-        <v>20.154225663343905</v>
+        <v>55.871054477305634</v>
       </c>
       <c r="C194">
-        <v>2.2009329928796837</v>
+        <v>2.2892079472910725</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -10112,39 +10112,39 @@
         <v>0</v>
       </c>
       <c r="H194">
-        <v>0.99871667878189552</v>
+        <v>1.1771465431440027</v>
       </c>
       <c r="I194">
-        <v>0</v>
+        <v>5.2857323993215521E-2</v>
       </c>
       <c r="J194">
-        <v>0.18023289885861621</v>
+        <v>0.19105532429335412</v>
       </c>
       <c r="K194">
-        <v>0.11059826005601686</v>
+        <v>0.10914556053477255</v>
       </c>
       <c r="L194">
         <v>0</v>
       </c>
       <c r="M194">
-        <v>0.1153712820957727</v>
+        <v>7.9577475710236087E-2</v>
       </c>
       <c r="N194">
         <v>0</v>
       </c>
       <c r="O194">
-        <v>3.8226896167542002</v>
-      </c>
-    </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.8459377758916378</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B195">
-        <v>55.871054477305634</v>
+        <v>43.816543767660242</v>
       </c>
       <c r="C195">
-        <v>2.2892079472910725</v>
+        <v>2.9758908519384231</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -10159,39 +10159,39 @@
         <v>0</v>
       </c>
       <c r="H195">
-        <v>1.1771465431440027</v>
+        <v>1.3509713570173101</v>
       </c>
       <c r="I195">
-        <v>5.2857323993215521E-2</v>
+        <v>0.20697361160318489</v>
       </c>
       <c r="J195">
-        <v>0.19105532429335412</v>
+        <v>0.28727032601998298</v>
       </c>
       <c r="K195">
-        <v>0.10914556053477255</v>
+        <v>0.20538777577806824</v>
       </c>
       <c r="L195">
-        <v>0</v>
+        <v>0.21104183805035456</v>
       </c>
       <c r="M195">
-        <v>7.9577475710236087E-2</v>
+        <v>0.26649519386978227</v>
       </c>
       <c r="N195">
         <v>0</v>
       </c>
       <c r="O195">
-        <v>3.8459377758916378</v>
-      </c>
-    </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.8759988120263404</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B196">
-        <v>43.816543767660242</v>
+        <v>45.630878852307454</v>
       </c>
       <c r="C196">
-        <v>2.9758908519384231</v>
+        <v>2.8920319519955546</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -10206,39 +10206,39 @@
         <v>0</v>
       </c>
       <c r="H196">
-        <v>1.3509713570173101</v>
+        <v>1.9662366016695687</v>
       </c>
       <c r="I196">
-        <v>0.20697361160318489</v>
+        <v>0.37234550549106332</v>
       </c>
       <c r="J196">
-        <v>0.28727032601998298</v>
+        <v>0.51338679852554636</v>
       </c>
       <c r="K196">
-        <v>0.20538777577806824</v>
+        <v>0.26252518074207654</v>
       </c>
       <c r="L196">
-        <v>0.21104183805035456</v>
+        <v>0.31115991053930031</v>
       </c>
       <c r="M196">
-        <v>0.26649519386978227</v>
+        <v>0.67559057446953263</v>
       </c>
       <c r="N196">
         <v>0</v>
       </c>
       <c r="O196">
-        <v>3.8759988120263404</v>
-      </c>
-    </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4.309191727635227</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B197">
-        <v>45.630878852307454</v>
+        <v>47.988593521116535</v>
       </c>
       <c r="C197">
-        <v>2.8920319519955546</v>
+        <v>1.7356245141872702</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -10253,39 +10253,39 @@
         <v>0</v>
       </c>
       <c r="H197">
-        <v>1.9662366016695687</v>
+        <v>2.4592158224115721</v>
       </c>
       <c r="I197">
-        <v>0.37234550549106332</v>
+        <v>0.42606201804089017</v>
       </c>
       <c r="J197">
-        <v>0.51338679852554636</v>
+        <v>0.53260454256173861</v>
       </c>
       <c r="K197">
-        <v>0.26252518074207654</v>
+        <v>0.33025627131012353</v>
       </c>
       <c r="L197">
-        <v>0.31115991053930031</v>
+        <v>0.4767965521286498</v>
       </c>
       <c r="M197">
-        <v>0.67559057446953263</v>
+        <v>0.84683499811355145</v>
       </c>
       <c r="N197">
         <v>0</v>
       </c>
       <c r="O197">
-        <v>4.309191727635227</v>
-      </c>
-    </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.7634164215770829</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B198">
-        <v>47.988593521116535</v>
+        <v>0</v>
       </c>
       <c r="C198">
-        <v>1.7356245141872702</v>
+        <v>0</v>
       </c>
       <c r="D198">
         <v>0</v>
@@ -10300,33 +10300,33 @@
         <v>0</v>
       </c>
       <c r="H198">
-        <v>2.4592158224115721</v>
+        <v>0</v>
       </c>
       <c r="I198">
-        <v>0.42606201804089017</v>
+        <v>0</v>
       </c>
       <c r="J198">
-        <v>0.53260454256173861</v>
+        <v>0</v>
       </c>
       <c r="K198">
-        <v>0.33025627131012353</v>
+        <v>0</v>
       </c>
       <c r="L198">
-        <v>0.4767965521286498</v>
+        <v>0</v>
       </c>
       <c r="M198">
-        <v>0.84683499811355145</v>
+        <v>0</v>
       </c>
       <c r="N198">
         <v>0</v>
       </c>
       <c r="O198">
-        <v>3.7634164215770829</v>
-      </c>
-    </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.18912118656579155</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -10368,15 +10368,15 @@
         <v>0</v>
       </c>
       <c r="O199">
-        <v>0.18912118656579155</v>
-      </c>
-    </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.3016162993495049</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B200">
-        <v>0</v>
+        <v>30.71722205423734</v>
       </c>
       <c r="C200">
         <v>0</v>
@@ -10415,18 +10415,18 @@
         <v>0</v>
       </c>
       <c r="O200">
-        <v>0.3016162993495049</v>
-      </c>
-    </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0.5922641009594678</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B201">
-        <v>30.71722205423734</v>
+        <v>28.073410006153523</v>
       </c>
       <c r="C201">
-        <v>0</v>
+        <v>3.0803275535077113E-2</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -10441,7 +10441,7 @@
         <v>0</v>
       </c>
       <c r="H201">
-        <v>0</v>
+        <v>0.41926266621775354</v>
       </c>
       <c r="I201">
         <v>0</v>
@@ -10462,18 +10462,18 @@
         <v>0</v>
       </c>
       <c r="O201">
-        <v>0.5922641009594678</v>
-      </c>
-    </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1.1816937731692321</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B202">
-        <v>28.073410006153523</v>
+        <v>26.381952311914045</v>
       </c>
       <c r="C202">
-        <v>3.0803275535077113E-2</v>
+        <v>0.18953931778532318</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -10488,7 +10488,7 @@
         <v>0</v>
       </c>
       <c r="H202">
-        <v>0.41926266621775354</v>
+        <v>0.66511866970724265</v>
       </c>
       <c r="I202">
         <v>0</v>
@@ -10509,18 +10509,18 @@
         <v>0</v>
       </c>
       <c r="O202">
-        <v>1.1816937731692321</v>
-      </c>
-    </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.45">
+        <v>2.0753642015315914</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B203">
-        <v>26.381952311914045</v>
+        <v>25.045296948273563</v>
       </c>
       <c r="C203">
-        <v>0.18953931778532318</v>
+        <v>0.43940395617208799</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -10535,13 +10535,13 @@
         <v>0</v>
       </c>
       <c r="H203">
-        <v>0.66511866970724265</v>
+        <v>0.91293844493479281</v>
       </c>
       <c r="I203">
         <v>0</v>
       </c>
       <c r="J203">
-        <v>0</v>
+        <v>0.11202242405095937</v>
       </c>
       <c r="K203">
         <v>0</v>
@@ -10556,18 +10556,18 @@
         <v>0</v>
       </c>
       <c r="O203">
-        <v>2.0753642015315914</v>
-      </c>
-    </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.4673153872867575</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B204">
-        <v>25.045296948273563</v>
+        <v>21.762418838575016</v>
       </c>
       <c r="C204">
-        <v>0.43940395617208799</v>
+        <v>1.2233611120423036</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -10582,39 +10582,39 @@
         <v>0</v>
       </c>
       <c r="H204">
-        <v>0.91293844493479281</v>
+        <v>1.214030853467944</v>
       </c>
       <c r="I204">
         <v>0</v>
       </c>
       <c r="J204">
-        <v>0.11202242405095937</v>
+        <v>0.10424138322565431</v>
       </c>
       <c r="K204">
-        <v>0</v>
+        <v>0.22817472397633792</v>
       </c>
       <c r="L204">
-        <v>0</v>
+        <v>0.20567206691260745</v>
       </c>
       <c r="M204">
-        <v>0</v>
+        <v>8.4189473276039331E-2</v>
       </c>
       <c r="N204">
         <v>0</v>
       </c>
       <c r="O204">
-        <v>3.4673153872867575</v>
-      </c>
-    </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4.5693894288319381</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B205">
-        <v>21.762418838575016</v>
+        <v>56.33283154570185</v>
       </c>
       <c r="C205">
-        <v>1.2233611120423036</v>
+        <v>1.3553468317047028</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -10629,39 +10629,39 @@
         <v>0</v>
       </c>
       <c r="H205">
-        <v>1.214030853467944</v>
+        <v>1.101350214213054</v>
       </c>
       <c r="I205">
-        <v>0</v>
+        <v>4.2087376212465673E-2</v>
       </c>
       <c r="J205">
-        <v>0.10424138322565431</v>
+        <v>0.32505542545760785</v>
       </c>
       <c r="K205">
-        <v>0.22817472397633792</v>
+        <v>0.13721191055932067</v>
       </c>
       <c r="L205">
-        <v>0.20567206691260745</v>
+        <v>0.21879276888309881</v>
       </c>
       <c r="M205">
-        <v>8.4189473276039331E-2</v>
+        <v>0</v>
       </c>
       <c r="N205">
         <v>0</v>
       </c>
       <c r="O205">
-        <v>4.5693894288319381</v>
-      </c>
-    </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4.366179617970336</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B206">
-        <v>56.33283154570185</v>
+        <v>48.916254618077204</v>
       </c>
       <c r="C206">
-        <v>1.3553468317047028</v>
+        <v>1.2737925974662152</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -10676,39 +10676,39 @@
         <v>0</v>
       </c>
       <c r="H206">
-        <v>1.101350214213054</v>
+        <v>1.2043134272409395</v>
       </c>
       <c r="I206">
-        <v>4.2087376212465673E-2</v>
+        <v>0.16195263216014352</v>
       </c>
       <c r="J206">
-        <v>0.32505542545760785</v>
+        <v>0.39219481207733198</v>
       </c>
       <c r="K206">
-        <v>0.13721191055932067</v>
+        <v>0.3009883711507868</v>
       </c>
       <c r="L206">
-        <v>0.21879276888309881</v>
+        <v>0.44396369146214665</v>
       </c>
       <c r="M206">
-        <v>0</v>
+        <v>0.19471997334958671</v>
       </c>
       <c r="N206">
         <v>0</v>
       </c>
       <c r="O206">
-        <v>4.366179617970336</v>
-      </c>
-    </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4.522060750442594</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B207">
-        <v>48.916254618077204</v>
+        <v>52.28496147586813</v>
       </c>
       <c r="C207">
-        <v>1.2737925974662152</v>
+        <v>0.71854627416972372</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -10723,39 +10723,39 @@
         <v>0</v>
       </c>
       <c r="H207">
-        <v>1.2043134272409395</v>
+        <v>1.2998182287158897</v>
       </c>
       <c r="I207">
-        <v>0.16195263216014352</v>
+        <v>0.26729175023664231</v>
       </c>
       <c r="J207">
-        <v>0.39219481207733198</v>
+        <v>0.44931189297059793</v>
       </c>
       <c r="K207">
-        <v>0.3009883711507868</v>
+        <v>0.3959185423599948</v>
       </c>
       <c r="L207">
-        <v>0.44396369146214665</v>
+        <v>0.89179514276963046</v>
       </c>
       <c r="M207">
-        <v>0.19471997334958671</v>
+        <v>0.43046814723809879</v>
       </c>
       <c r="N207">
         <v>0</v>
       </c>
       <c r="O207">
-        <v>4.522060750442594</v>
-      </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.45">
+        <v>3.9445052514132342</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B208">
-        <v>52.28496147586813</v>
+        <v>48.814065435851816</v>
       </c>
       <c r="C208">
-        <v>0.71854627416972372</v>
+        <v>0.37730400981341072</v>
       </c>
       <c r="D208">
         <v>0</v>
@@ -10770,74 +10770,27 @@
         <v>0</v>
       </c>
       <c r="H208">
-        <v>1.2998182287158897</v>
+        <v>1.3686017082429383</v>
       </c>
       <c r="I208">
-        <v>0.26729175023664231</v>
+        <v>0.24591115913729458</v>
       </c>
       <c r="J208">
-        <v>0.44931189297059793</v>
+        <v>0.50770737080541706</v>
       </c>
       <c r="K208">
-        <v>0.3959185423599948</v>
+        <v>0.51635186646277198</v>
       </c>
       <c r="L208">
-        <v>0.89179514276963046</v>
+        <v>0.86574385461561854</v>
       </c>
       <c r="M208">
-        <v>0.43046814723809879</v>
+        <v>0.91745650805223644</v>
       </c>
       <c r="N208">
         <v>0</v>
       </c>
       <c r="O208">
-        <v>3.9445052514132342</v>
-      </c>
-    </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A209" t="s">
-        <v>222</v>
-      </c>
-      <c r="B209">
-        <v>48.814065435851816</v>
-      </c>
-      <c r="C209">
-        <v>0.37730400981341072</v>
-      </c>
-      <c r="D209">
-        <v>0</v>
-      </c>
-      <c r="E209">
-        <v>0</v>
-      </c>
-      <c r="F209">
-        <v>0</v>
-      </c>
-      <c r="G209">
-        <v>0</v>
-      </c>
-      <c r="H209">
-        <v>1.3686017082429383</v>
-      </c>
-      <c r="I209">
-        <v>0.24591115913729458</v>
-      </c>
-      <c r="J209">
-        <v>0.50770737080541706</v>
-      </c>
-      <c r="K209">
-        <v>0.51635186646277198</v>
-      </c>
-      <c r="L209">
-        <v>0.86574385461561854</v>
-      </c>
-      <c r="M209">
-        <v>0.91745650805223644</v>
-      </c>
-      <c r="N209">
-        <v>0</v>
-      </c>
-      <c r="O209">
         <v>4.3433607179449378</v>
       </c>
     </row>
@@ -10853,7 +10806,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>